<commit_message>
Added BRK.B, PAYC, updated TTD models
</commit_message>
<xml_diff>
--- a/Industrials/Waste Management.xlsx
+++ b/Industrials/Waste Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Value/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Industrials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA14706F-BF2F-E14C-831C-4D5D6290CBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A707B63-2285-8341-AADD-EB2C5402B4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="27100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28380" yWindow="500" windowWidth="22800" windowHeight="27100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -646,7 +646,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,6 +685,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,10 +906,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -919,19 +921,6 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="39" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="16" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -973,6 +962,18 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -985,18 +986,25 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="10" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="39" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,7 +1097,7 @@
           <c:x val="7.932338308457712E-2"/>
           <c:y val="0.12583290202955646"/>
           <c:w val="0.87158872305140966"/>
-          <c:h val="0.75197121738212847"/>
+          <c:h val="0.68839147225234465"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1671,6 +1679,7 @@
         <c:axId val="248270543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1704,7 +1713,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -2653,10 +2662,10 @@
   <dimension ref="A1:AT118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AH65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AO79" sqref="AO79"/>
+      <selection pane="bottomRight" activeCell="AM29" sqref="AM29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2778,19 +2787,19 @@
       <c r="AK1" s="8">
         <v>2022</v>
       </c>
-      <c r="AL1" s="27">
+      <c r="AL1" s="25">
         <v>2023</v>
       </c>
-      <c r="AM1" s="27">
+      <c r="AM1" s="25">
         <v>2024</v>
       </c>
-      <c r="AN1" s="27">
+      <c r="AN1" s="25">
         <v>2025</v>
       </c>
-      <c r="AO1" s="27">
+      <c r="AO1" s="25">
         <v>2026</v>
       </c>
-      <c r="AP1" s="27">
+      <c r="AP1" s="25">
         <v>2027</v>
       </c>
     </row>
@@ -3030,19 +3039,19 @@
       <c r="AK3" s="1">
         <v>19698000000</v>
       </c>
-      <c r="AL3" s="28">
+      <c r="AL3" s="26">
         <v>20678000000</v>
       </c>
-      <c r="AM3" s="28">
+      <c r="AM3" s="26">
         <v>21734000000</v>
       </c>
-      <c r="AN3" s="28">
+      <c r="AN3" s="26">
         <v>23201000000</v>
       </c>
-      <c r="AO3" s="28">
+      <c r="AO3" s="26">
         <v>24617000000</v>
       </c>
-      <c r="AP3" s="28">
+      <c r="AP3" s="26">
         <v>25905000000</v>
       </c>
       <c r="AQ3" s="18" t="s">
@@ -4763,19 +4772,19 @@
       <c r="AK16" s="1">
         <v>14232000000</v>
       </c>
-      <c r="AQ16" s="29">
+      <c r="AQ16" s="27">
         <f>(AK35+AJ35+AI35+AH35+AG35)/5</f>
         <v>-1.2439682651333278E-2</v>
       </c>
-      <c r="AR16" s="30">
+      <c r="AR16" s="28">
         <f>AS101/AK3</f>
         <v>3.1209259823332318</v>
       </c>
-      <c r="AS16" s="30">
+      <c r="AS16" s="28">
         <f>AS101/AK28</f>
         <v>27.469168900804288</v>
       </c>
-      <c r="AT16" s="31">
+      <c r="AT16" s="29">
         <f>AS101/AK106</f>
         <v>31.54232939969215</v>
       </c>
@@ -5121,10 +5130,7 @@
       <c r="AK19" s="10">
         <v>5332000000</v>
       </c>
-      <c r="AL19" s="32">
-        <v>5900000000</v>
-      </c>
-      <c r="AQ19" s="66">
+      <c r="AQ19" s="49">
         <f>AK40-AK56-AK61</f>
         <v>-14633000000</v>
       </c>
@@ -5274,10 +5280,6 @@
         <f t="shared" ref="AK20:AL20" si="8">(AK19/AJ19)-1</f>
         <v>0.13157894736842102</v>
       </c>
-      <c r="AL20" s="16">
-        <f t="shared" si="8"/>
-        <v>0.10652663165791454</v>
-      </c>
     </row>
     <row r="21" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -5391,10 +5393,6 @@
       <c r="AK21" s="2">
         <v>0.2707</v>
       </c>
-      <c r="AL21" s="2">
-        <f>AL19/AL3</f>
-        <v>0.28532740110262117</v>
-      </c>
     </row>
     <row r="22" spans="1:43" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -12503,10 +12501,10 @@
       <c r="AK83" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR83" s="60" t="s">
+      <c r="AR83" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="AS83" s="61"/>
+      <c r="AS83" s="54"/>
     </row>
     <row r="84" spans="1:45" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -12620,10 +12618,10 @@
       <c r="AK84" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR84" s="62" t="s">
+      <c r="AR84" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="AS84" s="63"/>
+      <c r="AS84" s="56"/>
     </row>
     <row r="85" spans="1:45" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -12737,10 +12735,10 @@
       <c r="AK85" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR85" s="23" t="s">
+      <c r="AR85" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="AS85" s="24">
+      <c r="AS85" s="58">
         <f>AK17</f>
         <v>378000000</v>
       </c>
@@ -12857,10 +12855,10 @@
       <c r="AK86" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR86" s="23" t="s">
+      <c r="AR86" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="AS86" s="24">
+      <c r="AS86" s="58">
         <f>AK56</f>
         <v>414000000</v>
       </c>
@@ -12977,10 +12975,10 @@
       <c r="AK87" s="10">
         <v>4536000000</v>
       </c>
-      <c r="AR87" s="23" t="s">
+      <c r="AR87" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="AS87" s="24">
+      <c r="AS87" s="58">
         <f>AK61</f>
         <v>14570000000</v>
       </c>
@@ -13097,10 +13095,10 @@
       <c r="AK88" s="1">
         <v>0</v>
       </c>
-      <c r="AR88" s="33" t="s">
+      <c r="AR88" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="AS88" s="34">
+      <c r="AS88" s="60">
         <f>AS85/(AS86+AS87)</f>
         <v>2.5226908702616124E-2</v>
       </c>
@@ -13253,10 +13251,10 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="AR89" s="23" t="s">
+      <c r="AR89" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="AS89" s="24">
+      <c r="AS89" s="58">
         <f>AK27</f>
         <v>678000000</v>
       </c>
@@ -13373,10 +13371,10 @@
       <c r="AK90" s="1">
         <v>-377000000</v>
       </c>
-      <c r="AR90" s="23" t="s">
+      <c r="AR90" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="AS90" s="24">
+      <c r="AS90" s="58">
         <f>AK25</f>
         <v>2918000000</v>
       </c>
@@ -13493,10 +13491,10 @@
       <c r="AK91" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR91" s="33" t="s">
+      <c r="AR91" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="AS91" s="34">
+      <c r="AS91" s="60">
         <f>AS89/AS90</f>
         <v>0.23235092529129542</v>
       </c>
@@ -13613,10 +13611,10 @@
       <c r="AK92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR92" s="35" t="s">
+      <c r="AR92" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="AS92" s="36">
+      <c r="AS92" s="62">
         <f>AS88*(1-AS91)</f>
         <v>1.9365413123324234E-2</v>
       </c>
@@ -13733,10 +13731,10 @@
       <c r="AK93" s="1">
         <v>-2686000000</v>
       </c>
-      <c r="AR93" s="62" t="s">
+      <c r="AR93" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="AS93" s="63"/>
+      <c r="AS93" s="56"/>
     </row>
     <row r="94" spans="1:45" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -13850,10 +13848,10 @@
       <c r="AK94" s="10">
         <v>-3063000000</v>
       </c>
-      <c r="AR94" s="23" t="s">
+      <c r="AR94" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="AS94" s="37">
+      <c r="AS94" s="63">
         <v>4.095E-2</v>
       </c>
     </row>
@@ -13969,10 +13967,10 @@
       <c r="AK95" s="1">
         <v>-7328000000</v>
       </c>
-      <c r="AR95" s="23" t="s">
+      <c r="AR95" s="65" t="s">
         <v>136</v>
       </c>
-      <c r="AS95" s="38">
+      <c r="AS95" s="66">
         <v>0.73</v>
       </c>
     </row>
@@ -14088,10 +14086,10 @@
       <c r="AK96" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AR96" s="23" t="s">
+      <c r="AR96" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="AS96" s="37">
+      <c r="AS96" s="63">
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
@@ -14207,10 +14205,10 @@
       <c r="AK97" s="1">
         <v>-1500000000</v>
       </c>
-      <c r="AR97" s="35" t="s">
+      <c r="AR97" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="AS97" s="36">
+      <c r="AS97" s="62">
         <f>(AS94)+((AS95)*(AS96-AS94))</f>
         <v>7.237650000000001E-2</v>
       </c>
@@ -14327,10 +14325,10 @@
       <c r="AK98" s="1">
         <v>-1077000000</v>
       </c>
-      <c r="AR98" s="62" t="s">
+      <c r="AR98" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="AS98" s="63"/>
+      <c r="AS98" s="56"/>
     </row>
     <row r="99" spans="1:45" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -14444,10 +14442,10 @@
       <c r="AK99" s="1">
         <v>8689000000</v>
       </c>
-      <c r="AR99" s="23" t="s">
+      <c r="AR99" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="AS99" s="24">
+      <c r="AS99" s="58">
         <f>AS86+AS87</f>
         <v>14984000000</v>
       </c>
@@ -14564,10 +14562,10 @@
       <c r="AK100" s="10">
         <v>-1216000000</v>
       </c>
-      <c r="AR100" s="33" t="s">
+      <c r="AR100" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="AS100" s="34">
+      <c r="AS100" s="60">
         <f>AS99/AS103</f>
         <v>0.19597174993460634</v>
       </c>
@@ -14684,10 +14682,10 @@
       <c r="AK101" s="1">
         <v>-6000000</v>
       </c>
-      <c r="AR101" s="23" t="s">
+      <c r="AR101" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="AS101" s="39">
+      <c r="AS101" s="67">
         <v>61476000000</v>
       </c>
     </row>
@@ -14803,10 +14801,10 @@
       <c r="AK102" s="10">
         <v>251000000</v>
       </c>
-      <c r="AR102" s="33" t="s">
+      <c r="AR102" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="AS102" s="34">
+      <c r="AS102" s="60">
         <f>AS101/AS103</f>
         <v>0.80402825006539369</v>
       </c>
@@ -14923,10 +14921,10 @@
       <c r="AK103" s="1">
         <v>194000000</v>
       </c>
-      <c r="AR103" s="35" t="s">
+      <c r="AR103" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="AS103" s="40">
+      <c r="AS103" s="64">
         <f>AS99+AS101</f>
         <v>76460000000</v>
       </c>
@@ -15043,10 +15041,10 @@
       <c r="AK104" s="11">
         <v>445000000</v>
       </c>
-      <c r="AR104" s="62" t="s">
+      <c r="AR104" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="AS104" s="63"/>
+      <c r="AS104" s="56"/>
     </row>
     <row r="105" spans="1:45" ht="20" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
@@ -15199,10 +15197,10 @@
       <c r="AO105" s="15"/>
       <c r="AP105" s="15"/>
       <c r="AQ105" s="15"/>
-      <c r="AR105" s="25" t="s">
+      <c r="AR105" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="AS105" s="26">
+      <c r="AS105" s="24">
         <f>(AS100*AS92)+(AS102*AS97)</f>
         <v>6.1987824538842412E-2</v>
       </c>
@@ -15319,33 +15317,33 @@
       <c r="AK106" s="1">
         <v>1949000000</v>
       </c>
-      <c r="AL106" s="41">
+      <c r="AL106" s="30">
         <f>AK106*(1+$AS$106)</f>
         <v>2058795496.3247435</v>
       </c>
-      <c r="AM106" s="41">
+      <c r="AM106" s="30">
         <f t="shared" ref="AM106:AP106" si="29">AL106*(1+$AS$106)</f>
         <v>2174776242.0149035</v>
       </c>
-      <c r="AN106" s="41">
+      <c r="AN106" s="30">
         <f t="shared" si="29"/>
         <v>2297290678.5912437</v>
       </c>
-      <c r="AO106" s="41">
+      <c r="AO106" s="30">
         <f t="shared" si="29"/>
         <v>2426706876.7739697</v>
       </c>
-      <c r="AP106" s="41">
+      <c r="AP106" s="30">
         <f t="shared" si="29"/>
         <v>2563413642.2793908</v>
       </c>
-      <c r="AQ106" s="42" t="s">
+      <c r="AQ106" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="AR106" s="43" t="s">
+      <c r="AR106" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="AS106" s="44">
+      <c r="AS106" s="33">
         <f>(SUM(AL4:AP4)/5)</f>
         <v>5.6334272100945881E-2</v>
       </c>
@@ -15388,138 +15386,138 @@
       <c r="AI107" s="13"/>
       <c r="AJ107" s="13"/>
       <c r="AK107" s="13"/>
-      <c r="AL107" s="42"/>
-      <c r="AM107" s="42"/>
-      <c r="AN107" s="42"/>
-      <c r="AO107" s="42"/>
-      <c r="AP107" s="45">
+      <c r="AL107" s="31"/>
+      <c r="AM107" s="31"/>
+      <c r="AN107" s="31"/>
+      <c r="AO107" s="31"/>
+      <c r="AP107" s="34">
         <f>AP106*(1+AS107)/(AS108-AS107)</f>
-        <v>62272383574.104187</v>
-      </c>
-      <c r="AQ107" s="46" t="s">
+        <v>71036861888.893524</v>
+      </c>
+      <c r="AQ107" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="AR107" s="47" t="s">
+      <c r="AR107" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="AS107" s="48">
-        <v>0.02</v>
+      <c r="AS107" s="37">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:45" ht="19" x14ac:dyDescent="0.25">
-      <c r="AL108" s="45">
+      <c r="AL108" s="34">
         <f t="shared" ref="AL108:AN108" si="30">AL107+AL106</f>
         <v>2058795496.3247435</v>
       </c>
-      <c r="AM108" s="45">
+      <c r="AM108" s="34">
         <f t="shared" si="30"/>
         <v>2174776242.0149035</v>
       </c>
-      <c r="AN108" s="45">
+      <c r="AN108" s="34">
         <f t="shared" si="30"/>
         <v>2297290678.5912437</v>
       </c>
-      <c r="AO108" s="45">
+      <c r="AO108" s="34">
         <f>AO107+AO106</f>
         <v>2426706876.7739697</v>
       </c>
-      <c r="AP108" s="45">
+      <c r="AP108" s="34">
         <f>AP107+AP106</f>
-        <v>64835797216.383575</v>
-      </c>
-      <c r="AQ108" s="46" t="s">
+        <v>73600275531.172913</v>
+      </c>
+      <c r="AQ108" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="AR108" s="49" t="s">
+      <c r="AR108" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="AS108" s="50">
+      <c r="AS108" s="39">
         <f>AS105</f>
         <v>6.1987824538842412E-2</v>
       </c>
     </row>
     <row r="109" spans="1:45" ht="19" x14ac:dyDescent="0.25">
-      <c r="AL109" s="64" t="s">
+      <c r="AL109" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AM109" s="65"/>
+      <c r="AM109" s="52"/>
     </row>
     <row r="110" spans="1:45" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL110" s="51" t="s">
+      <c r="AL110" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="AM110" s="52">
+      <c r="AM110" s="41">
         <f>NPV(AS108,AL108,AM108,AN108,AO108,AP108)</f>
-        <v>55690134464.223488</v>
+        <v>62178396520.795525</v>
       </c>
     </row>
     <row r="111" spans="1:45" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL111" s="51" t="s">
+      <c r="AL111" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="AM111" s="52">
+      <c r="AM111" s="41">
         <f>AK40</f>
         <v>351000000</v>
       </c>
     </row>
     <row r="112" spans="1:45" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL112" s="51" t="s">
+      <c r="AL112" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="AM112" s="52">
+      <c r="AM112" s="41">
         <f>AS99</f>
         <v>14984000000</v>
       </c>
     </row>
     <row r="113" spans="38:39" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL113" s="51" t="s">
+      <c r="AL113" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="AM113" s="52">
+      <c r="AM113" s="41">
         <f>AM110+AM111-AM112</f>
-        <v>41057134464.223488</v>
+        <v>47545396520.795525</v>
       </c>
     </row>
     <row r="114" spans="38:39" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL114" s="51" t="s">
+      <c r="AL114" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="AM114" s="67">
+      <c r="AM114" s="50">
         <f>AK34*(1+(5*AQ16))</f>
         <v>389187658.49848342</v>
       </c>
     </row>
     <row r="115" spans="38:39" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL115" s="54" t="s">
+      <c r="AL115" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="AM115" s="55">
+      <c r="AM115" s="44">
         <f>AM113/AM114</f>
-        <v>105.49444096615278</v>
+        <v>122.1657354301249</v>
       </c>
     </row>
     <row r="116" spans="38:39" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL116" s="53" t="s">
+      <c r="AL116" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="AM116" s="56">
+      <c r="AM116" s="45">
         <v>150.62</v>
       </c>
     </row>
     <row r="117" spans="38:39" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL117" s="57" t="s">
+      <c r="AL117" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="AM117" s="58">
+      <c r="AM117" s="47">
         <f>AM115/AM116-1</f>
-        <v>-0.29959871885438338</v>
+        <v>-0.18891425155938857</v>
       </c>
     </row>
     <row r="118" spans="38:39" ht="20" x14ac:dyDescent="0.25">
-      <c r="AL118" s="57" t="s">
+      <c r="AL118" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="AM118" s="59" t="str">
+      <c r="AM118" s="48" t="str">
         <f>IF(AM115&gt;AM116,"BUY","SELL")</f>
         <v>SELL</v>
       </c>

</xml_diff>